<commit_message>
POITEM Vendor Class PO Loader Change in Connection name for some of the TC
</commit_message>
<xml_diff>
--- a/templates/RSTKF_AutomationData.xlsx
+++ b/templates/RSTKF_AutomationData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dellDevonforce\Provar\ERPFinalProj\rsqasampleproj\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FE05260-664D-4140-8303-6EF0B7CC4C2F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E3ABC23-45E7-4228-B788-277DA0EB2A91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="3" activeTab="4" xr2:uid="{B6C21A89-21B4-4624-A955-66D166717697}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="10" activeTab="13" xr2:uid="{B6C21A89-21B4-4624-A955-66D166717697}"/>
   </bookViews>
   <sheets>
     <sheet name="PurchaseOrder" sheetId="3" r:id="rId1"/>
@@ -25,7 +25,9 @@
     <sheet name="POAuthorizationPartial" sheetId="14" r:id="rId10"/>
     <sheet name="PurchaseRequisition" sheetId="9" r:id="rId11"/>
     <sheet name="InventoryRequisition" sheetId="10" r:id="rId12"/>
-    <sheet name="IndirectRequisition" sheetId="11" r:id="rId13"/>
+    <sheet name="VendorClass" sheetId="15" r:id="rId13"/>
+    <sheet name="NONINVPOITEM" sheetId="16" r:id="rId14"/>
+    <sheet name="IndirectRequisition" sheetId="11" r:id="rId15"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -46,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="82">
   <si>
     <t>Vendor</t>
   </si>
@@ -184,13 +186,121 @@
   </si>
   <si>
     <t>NPAuto_Purchased_SRL (Purchased serial for automation)</t>
+  </si>
+  <si>
+    <t>il…</t>
+  </si>
+  <si>
+    <t>PO Price Override</t>
+  </si>
+  <si>
+    <t>Namrata Patil</t>
+  </si>
+  <si>
+    <t>Responsible</t>
+  </si>
+  <si>
+    <t>Create_Buyer</t>
+  </si>
+  <si>
+    <t>Create_Payterms</t>
+  </si>
+  <si>
+    <t>Create_APUser</t>
+  </si>
+  <si>
+    <t>Create_glacct</t>
+  </si>
+  <si>
+    <t>Create_BankName</t>
+  </si>
+  <si>
+    <t>Create_paytype</t>
+  </si>
+  <si>
+    <t>Edit_paytype</t>
+  </si>
+  <si>
+    <t>Edit_glacct</t>
+  </si>
+  <si>
+    <t>Edit_BankName</t>
+  </si>
+  <si>
+    <t>210-N30 (2%-10, Net 30)</t>
+  </si>
+  <si>
+    <t>1094 (Interest Expense)</t>
+  </si>
+  <si>
+    <t>Check</t>
+  </si>
+  <si>
+    <t>4588 (COS - Standards Variance)</t>
+  </si>
+  <si>
+    <t>Central Bank Of India</t>
+  </si>
+  <si>
+    <t>Cash</t>
+  </si>
+  <si>
+    <t>BC-Bank</t>
+  </si>
+  <si>
+    <t>Edit_Freightterms</t>
+  </si>
+  <si>
+    <t>TEST1234</t>
+  </si>
+  <si>
+    <t>Edit_FOB</t>
+  </si>
+  <si>
+    <t>ORIGIN (Origin)</t>
+  </si>
+  <si>
+    <t>Edit_Carrier</t>
+  </si>
+  <si>
+    <t>UPS (UPS)</t>
+  </si>
+  <si>
+    <t>Edit_shippingmethod</t>
+  </si>
+  <si>
+    <t>Ground (Ground)</t>
+  </si>
+  <si>
+    <t>Create_ItemType</t>
+  </si>
+  <si>
+    <t>Create_POCommcod</t>
+  </si>
+  <si>
+    <t>Create_odc</t>
+  </si>
+  <si>
+    <t>Edit_ExpenseAcct</t>
+  </si>
+  <si>
+    <t>Indirect Material</t>
+  </si>
+  <si>
+    <t>PK_Buy_Indirect</t>
+  </si>
+  <si>
+    <t>raul-indirect MT</t>
+  </si>
+  <si>
+    <t>21.18 (Test Sub 21.18)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -209,6 +319,12 @@
       <color rgb="FF222222"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF222222"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="4">
@@ -243,7 +359,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -255,6 +371,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -758,18 +875,19 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8B3CC08-5902-46B1-B680-4FBFE135756B}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C3"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="51.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -779,8 +897,17 @@
       <c r="C1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -790,8 +917,14 @@
       <c r="C2">
         <v>23</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
@@ -800,6 +933,12 @@
       </c>
       <c r="C3">
         <v>50</v>
+      </c>
+      <c r="D3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -808,6 +947,156 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A6130D2-2258-4970-AEC9-AEEFF9FC83D2}">
+  <dimension ref="A1:M2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J1" t="s">
+        <v>72</v>
+      </c>
+      <c r="K1" t="s">
+        <v>57</v>
+      </c>
+      <c r="L1" t="s">
+        <v>58</v>
+      </c>
+      <c r="M1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F2" t="s">
+        <v>61</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4AC5DC2-E025-402D-BF69-1EF7E4D3E24B}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>81</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43030A8E-5EF5-4C2C-9F45-5AB5995C2560}">
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -1065,9 +1354,9 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC9C9AD3-2B09-4E34-AACF-6768C297C7C0}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
@@ -1077,7 +1366,7 @@
     <col min="3" max="3" width="37.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1094,7 +1383,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -1111,7 +1400,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>43</v>
       </c>
@@ -1125,7 +1414,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
@@ -1139,7 +1428,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>11</v>
       </c>
@@ -1151,6 +1440,11 @@
       </c>
       <c r="E5">
         <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G10" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
SYDATA TC'S POLOADER TC's
</commit_message>
<xml_diff>
--- a/templates/RSTKF_AutomationData.xlsx
+++ b/templates/RSTKF_AutomationData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dellDevonforce\Provar\ERPFinalProj\rsqasampleproj\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E3ABC23-45E7-4228-B788-277DA0EB2A91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1E462F9-C9B8-4066-A743-61C587639A91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="10" activeTab="13" xr2:uid="{B6C21A89-21B4-4624-A955-66D166717697}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="3" activeTab="4" xr2:uid="{B6C21A89-21B4-4624-A955-66D166717697}"/>
   </bookViews>
   <sheets>
     <sheet name="PurchaseOrder" sheetId="3" r:id="rId1"/>
@@ -27,7 +27,8 @@
     <sheet name="InventoryRequisition" sheetId="10" r:id="rId12"/>
     <sheet name="VendorClass" sheetId="15" r:id="rId13"/>
     <sheet name="NONINVPOITEM" sheetId="16" r:id="rId14"/>
-    <sheet name="IndirectRequisition" sheetId="11" r:id="rId15"/>
+    <sheet name="VendorMaster" sheetId="17" r:id="rId15"/>
+    <sheet name="IndirectRequisition" sheetId="11" r:id="rId16"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -48,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="91">
   <si>
     <t>Vendor</t>
   </si>
@@ -188,9 +189,6 @@
     <t>NPAuto_Purchased_SRL (Purchased serial for automation)</t>
   </si>
   <si>
-    <t>il…</t>
-  </si>
-  <si>
     <t>PO Price Override</t>
   </si>
   <si>
@@ -294,6 +292,36 @@
   </si>
   <si>
     <t>21.18 (Test Sub 21.18)</t>
+  </si>
+  <si>
+    <t>Street</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>Zip</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Avenue Villa</t>
+  </si>
+  <si>
+    <t>Boston</t>
+  </si>
+  <si>
+    <t>Massachusetts</t>
+  </si>
+  <si>
+    <t>US</t>
+  </si>
+  <si>
+    <t>Buyer</t>
   </si>
 </sst>
 </file>
@@ -901,10 +929,10 @@
         <v>37</v>
       </c>
       <c r="E1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -921,7 +949,7 @@
         <v>39</v>
       </c>
       <c r="E2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -938,7 +966,7 @@
         <v>39</v>
       </c>
       <c r="E3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -962,84 +990,84 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" t="s">
         <v>50</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>51</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>52</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>53</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>54</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H1" t="s">
+        <v>67</v>
+      </c>
+      <c r="I1" t="s">
+        <v>69</v>
+      </c>
+      <c r="J1" t="s">
+        <v>71</v>
+      </c>
+      <c r="K1" t="s">
+        <v>56</v>
+      </c>
+      <c r="L1" t="s">
+        <v>57</v>
+      </c>
+      <c r="M1" t="s">
         <v>55</v>
-      </c>
-      <c r="G1" t="s">
-        <v>66</v>
-      </c>
-      <c r="H1" t="s">
-        <v>68</v>
-      </c>
-      <c r="I1" t="s">
-        <v>70</v>
-      </c>
-      <c r="J1" t="s">
-        <v>72</v>
-      </c>
-      <c r="K1" t="s">
-        <v>57</v>
-      </c>
-      <c r="L1" t="s">
-        <v>58</v>
-      </c>
-      <c r="M1" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" t="s">
         <v>59</v>
       </c>
-      <c r="C2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F2" t="s">
         <v>60</v>
       </c>
-      <c r="E2" t="s">
-        <v>65</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="G2" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="K2" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="K2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>63</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -1052,7 +1080,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4AC5DC2-E025-402D-BF69-1EF7E4D3E24B}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
@@ -1064,30 +1092,30 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" t="s">
         <v>74</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>75</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>76</v>
-      </c>
-      <c r="D1" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B2" t="s">
         <v>78</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>79</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" s="7" t="s">
         <v>80</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -1097,6 +1125,64 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F6EF229-A232-4FA4-B9BE-B547E34B6D44}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2">
+        <v>2101</v>
+      </c>
+      <c r="F2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43030A8E-5EF5-4C2C-9F45-5AB5995C2560}">
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -1354,10 +1440,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC9C9AD3-2B09-4E34-AACF-6768C297C7C0}">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1366,7 +1452,7 @@
     <col min="3" max="3" width="37.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1383,7 +1469,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -1400,7 +1486,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>43</v>
       </c>
@@ -1414,7 +1500,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
@@ -1428,7 +1514,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>11</v>
       </c>
@@ -1440,11 +1526,6 @@
       </c>
       <c r="E5">
         <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G10" t="s">
-        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>